<commit_message>
Alaska Water Rights update
Alaska Water Rights update
</commit_message>
<xml_diff>
--- a/Alaska/WaterAllocation/AK_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Alaska/WaterAllocation/AK_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Alaska\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E78AAA-B96E-4FD5-B95D-DF2B709BED25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C36873A-B0F8-4B6D-A4DF-559160F65E5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="4" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="373">
   <si>
     <t>Name</t>
   </si>
@@ -1069,9 +1069,6 @@
     <t>WATER_SOURCE_ID</t>
   </si>
   <si>
-    <t>WATER_SOURCE_TYPE</t>
-  </si>
-  <si>
     <t>INTAKE_NAME</t>
   </si>
   <si>
@@ -1157,6 +1154,12 @@
   </si>
   <si>
     <t>https://dnr.alaska.gov/akwuds/</t>
+  </si>
+  <si>
+    <t>SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t>use Surface Water or Groundwater</t>
   </si>
 </sst>
 </file>
@@ -2593,7 +2596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2608,15 +2611,15 @@
         <v>236</v>
       </c>
       <c r="B1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B2" s="100" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2624,7 +2627,7 @@
         <v>237</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2637,12 +2640,12 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2650,17 +2653,17 @@
         <v>241</v>
       </c>
       <c r="B15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -2780,7 +2783,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="91" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F4" s="59" t="s">
         <v>38</v>
@@ -2812,7 +2815,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>38</v>
@@ -2844,7 +2847,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F6" s="44" t="s">
         <v>38</v>
@@ -2876,7 +2879,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>38</v>
@@ -2908,7 +2911,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F8" s="44" t="s">
         <v>38</v>
@@ -3002,7 +3005,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>38</v>
@@ -3034,7 +3037,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F12" s="44" t="s">
         <v>38</v>
@@ -3169,7 +3172,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="93" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>38</v>
@@ -3586,7 +3589,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>38</v>
@@ -3618,7 +3621,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="99" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>38</v>
@@ -3650,7 +3653,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F6" s="44" t="s">
         <v>38</v>
@@ -3682,7 +3685,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="99" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>38</v>
@@ -3714,7 +3717,7 @@
         <v>38</v>
       </c>
       <c r="E8" s="100" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F8" s="44" t="s">
         <v>38</v>
@@ -3746,7 +3749,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F9" s="44" t="s">
         <v>38</v>
@@ -3778,7 +3781,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F10" s="44" t="s">
         <v>38</v>
@@ -3810,7 +3813,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>38</v>
@@ -3842,7 +3845,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F12" s="44" t="s">
         <v>38</v>
@@ -3901,8 +3904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC5F405-0A84-4CAE-BAB0-9DF044EAE9B9}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3997,7 +4000,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F4" s="59" t="s">
         <v>38</v>
@@ -4027,7 +4030,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>38</v>
@@ -4057,7 +4060,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>38</v>
@@ -4177,13 +4180,13 @@
         <v>20</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>38</v>
+        <v>372</v>
       </c>
       <c r="F10" s="44" t="s">
         <v>338</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>342</v>
+        <v>371</v>
       </c>
       <c r="H10" s="81"/>
       <c r="I10" s="74" t="s">
@@ -4214,7 +4217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -4314,7 +4317,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F4" s="59"/>
       <c r="G4" s="65"/>
@@ -4340,7 +4343,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>38</v>
@@ -4370,7 +4373,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F6" s="44" t="s">
         <v>38</v>
@@ -4400,7 +4403,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>38</v>
@@ -4460,7 +4463,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F9" s="44" t="s">
         <v>38</v>
@@ -4488,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F10" s="44" t="s">
         <v>38</v>
@@ -4518,7 +4521,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>38</v>
@@ -4708,7 +4711,7 @@
       <c r="E18" s="23"/>
       <c r="F18" s="41"/>
       <c r="G18" s="31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H18" s="79"/>
       <c r="I18" s="78" t="s">
@@ -4732,7 +4735,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F19" s="44" t="s">
         <v>38</v>
@@ -4762,7 +4765,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F20" s="44" t="s">
         <v>38</v>
@@ -4792,7 +4795,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>38</v>
@@ -4822,7 +4825,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F22" s="44" t="s">
         <v>38</v>
@@ -4852,7 +4855,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F23" s="44" t="s">
         <v>38</v>
@@ -5139,7 +5142,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="66" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="31"/>
@@ -5167,7 +5170,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="102" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="31"/>
@@ -5195,7 +5198,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="31"/>
@@ -5223,7 +5226,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="31"/>
@@ -5251,7 +5254,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F13" s="59"/>
       <c r="G13" s="68"/>
@@ -5279,7 +5282,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>38</v>
@@ -5311,7 +5314,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>38</v>
@@ -5343,7 +5346,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F16" s="23" t="s">
         <v>38</v>
@@ -5375,7 +5378,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>38</v>
@@ -5407,7 +5410,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>38</v>
@@ -5439,7 +5442,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>38</v>
@@ -5471,7 +5474,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>38</v>
@@ -5503,7 +5506,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>38</v>
@@ -5535,7 +5538,7 @@
         <v>38</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F22" s="23" t="s">
         <v>38</v>
@@ -5573,7 +5576,7 @@
         <v>338</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H23" s="86" t="s">
         <v>38</v>
@@ -5695,7 +5698,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F27" s="23" t="s">
         <v>38</v>
@@ -5727,7 +5730,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="103" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>38</v>
@@ -5759,7 +5762,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="104" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F29" s="23" t="s">
         <v>38</v>
@@ -5791,7 +5794,7 @@
         <v>20</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F30" s="23" t="s">
         <v>38</v>
@@ -5885,7 +5888,7 @@
         <v>38</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F33" s="23" t="s">
         <v>38</v>
@@ -5917,7 +5920,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F34" s="23" t="s">
         <v>38</v>
@@ -5949,7 +5952,7 @@
         <v>20</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F35" s="23" t="s">
         <v>38</v>
@@ -6013,7 +6016,7 @@
         <v>38</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F37" s="23" t="s">
         <v>38</v>
@@ -6071,7 +6074,7 @@
         <v>38</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F39" s="23" t="s">
         <v>38</v>
@@ -6103,7 +6106,7 @@
         <v>38</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F40" s="23" t="s">
         <v>38</v>
@@ -6133,7 +6136,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F41" s="23" t="s">
         <v>38</v>
@@ -6165,7 +6168,7 @@
         <v>38</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F42" s="23" t="s">
         <v>38</v>
@@ -6197,7 +6200,7 @@
         <v>38</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F43" s="23" t="s">
         <v>38</v>
@@ -6229,7 +6232,7 @@
         <v>20</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F44" s="23" t="s">
         <v>38</v>
@@ -6293,7 +6296,7 @@
         <v>38</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F46" s="23" t="s">
         <v>38</v>

</xml_diff>